<commit_message>
Updates UX 2 data extraction
</commit_message>
<xml_diff>
--- a/docs/user study/results/UX 2.xlsx
+++ b/docs/user study/results/UX 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Varma\Documents\GitHub\MSAT-UI\docs\user study\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14B6C9A-A1CB-4BF1-9A31-88F705D8733C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F990C2E5-9D37-43B7-82FC-027D4C208334}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="74">
   <si>
     <t xml:space="preserve">How often do you do software development? </t>
   </si>
@@ -175,6 +175,81 @@
   </si>
   <si>
     <t>Follow Up ( 4 5 )</t>
+  </si>
+  <si>
+    <t>U9</t>
+  </si>
+  <si>
+    <t>U10</t>
+  </si>
+  <si>
+    <t>U11</t>
+  </si>
+  <si>
+    <t>U12</t>
+  </si>
+  <si>
+    <t>No ( Manual Testing )</t>
+  </si>
+  <si>
+    <t>User says importance to interace should be given same as functionality.</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>No. User felt this is not best way ( UI )to do the task.</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>NA ( protocol modified )</t>
+  </si>
+  <si>
+    <t>4 days in a week</t>
+  </si>
+  <si>
+    <t>No ( But familiar with the concept in his studies )</t>
+  </si>
+  <si>
+    <t>Both matters.</t>
+  </si>
+  <si>
+    <t>No. User felt it is time consuming.</t>
+  </si>
+  <si>
+    <t>Prefers all 3 combo</t>
+  </si>
+  <si>
+    <t>No. It depends on bug.</t>
+  </si>
+  <si>
+    <t>No. It depends.</t>
+  </si>
+  <si>
+    <t>No ( Use debugger usually )</t>
+  </si>
+  <si>
+    <t>Interface would be nice to have for better visualtion of existence of bugs.</t>
+  </si>
+  <si>
+    <t>P4 ( personal preference )</t>
+  </si>
+  <si>
+    <t>No. ( Uses debugger in general to find bugs )</t>
+  </si>
+  <si>
+    <t>Uses Visual Studio which is intuitive and easy to use.</t>
+  </si>
+  <si>
+    <t>No. User understood task differently.</t>
+  </si>
+  <si>
+    <t>No. ( *luxury of time )</t>
+  </si>
+  <si>
+    <t>No. Felt difficult to get to conclusion.</t>
   </si>
 </sst>
 </file>
@@ -502,32 +577,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="63.7109375" customWidth="1"/>
-    <col min="2" max="2" width="43.7109375" customWidth="1"/>
-    <col min="3" max="3" width="45.7109375" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" customWidth="1"/>
     <col min="4" max="4" width="31.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -540,8 +630,20 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -554,8 +656,20 @@
       <c r="D5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -568,8 +682,20 @@
       <c r="D7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -582,8 +708,20 @@
       <c r="D9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -595,6 +733,18 @@
       </c>
       <c r="D11" t="s">
         <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -604,10 +754,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{106BECBB-8D93-4A3B-AAAE-E4192AD3BAB2}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,27 +765,39 @@
     <col min="1" max="1" width="33.85546875" customWidth="1"/>
     <col min="2" max="2" width="30.140625" customWidth="1"/>
     <col min="3" max="3" width="38.28515625" customWidth="1"/>
-    <col min="4" max="4" width="59.5703125" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -648,13 +810,25 @@
       <c r="D4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -667,13 +841,25 @@
       <c r="D9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -686,26 +872,56 @@
       <c r="D13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
       <c r="B17" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" t="s">
+        <v>55</v>
+      </c>
+      <c r="H17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -718,8 +934,20 @@
       <c r="D21">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>10</v>
+      </c>
+      <c r="F21">
+        <v>9</v>
+      </c>
+      <c r="G21">
+        <v>9</v>
+      </c>
+      <c r="H21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -732,8 +960,20 @@
       <c r="D22">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>7</v>
+      </c>
+      <c r="F22">
+        <v>6</v>
+      </c>
+      <c r="G22">
+        <v>7</v>
+      </c>
+      <c r="H22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -746,13 +986,25 @@
       <c r="D23">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>8</v>
+      </c>
+      <c r="F23">
+        <v>7</v>
+      </c>
+      <c r="G23">
+        <v>9</v>
+      </c>
+      <c r="H23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -765,13 +1017,25 @@
       <c r="D28" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>20</v>
       </c>
@@ -784,26 +1048,59 @@
       <c r="D32" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" t="s">
+        <v>41</v>
+      </c>
+      <c r="D36" t="s">
+        <v>39</v>
+      </c>
+      <c r="E36" t="s">
+        <v>39</v>
+      </c>
+      <c r="F36" t="s">
+        <v>39</v>
+      </c>
+      <c r="G36" t="s">
+        <v>41</v>
+      </c>
+      <c r="H36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>30</v>
       </c>
@@ -816,8 +1113,20 @@
       <c r="D40">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>8</v>
+      </c>
+      <c r="F40">
+        <v>8</v>
+      </c>
+      <c r="G40">
+        <v>10</v>
+      </c>
+      <c r="H40">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>32</v>
       </c>
@@ -829,6 +1138,18 @@
       </c>
       <c r="D41">
         <v>6</v>
+      </c>
+      <c r="E41">
+        <v>10</v>
+      </c>
+      <c r="F41">
+        <v>10</v>
+      </c>
+      <c r="G41">
+        <v>9</v>
+      </c>
+      <c r="H41">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -839,10 +1160,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45323CDF-F889-4C6F-9670-4C878856AA6C}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -853,30 +1174,41 @@
     <col min="4" max="4" width="33.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
@@ -889,11 +1221,23 @@
       <c r="D5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -906,8 +1250,20 @@
       <c r="D7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>8</v>
+      </c>
+      <c r="F7">
+        <v>8</v>
+      </c>
+      <c r="G7">
+        <v>7</v>
+      </c>
+      <c r="H7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -920,8 +1276,20 @@
       <c r="D8">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>9</v>
+      </c>
+      <c r="G8">
+        <v>8</v>
+      </c>
+      <c r="H8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -934,16 +1302,28 @@
       <c r="D9">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9">
+        <v>9</v>
+      </c>
+      <c r="H9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>33</v>
       </c>
@@ -956,11 +1336,23 @@
       <c r="D15" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -973,8 +1365,20 @@
       <c r="D17">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>8</v>
+      </c>
+      <c r="F17">
+        <v>9</v>
+      </c>
+      <c r="G17">
+        <v>9</v>
+      </c>
+      <c r="H17">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -986,6 +1390,18 @@
       </c>
       <c r="D18">
         <v>6</v>
+      </c>
+      <c r="E18">
+        <v>10</v>
+      </c>
+      <c r="F18">
+        <v>6</v>
+      </c>
+      <c r="G18">
+        <v>9</v>
+      </c>
+      <c r="H18">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -995,10 +1411,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0454749A-2141-49B1-B678-977DE214E3EB}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,27 +1425,38 @@
     <col min="4" max="4" width="49.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1042,13 +1469,25 @@
       <c r="D5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -1061,13 +1500,25 @@
       <c r="D9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1080,13 +1531,25 @@
       <c r="D13" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" t="s">
+        <v>57</v>
+      </c>
+      <c r="H13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1099,8 +1562,20 @@
       <c r="D17">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>10</v>
+      </c>
+      <c r="F17">
+        <v>8</v>
+      </c>
+      <c r="G17">
+        <v>8</v>
+      </c>
+      <c r="H17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1113,13 +1588,25 @@
       <c r="D18">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>8</v>
+      </c>
+      <c r="F18">
+        <v>6</v>
+      </c>
+      <c r="G18">
+        <v>10</v>
+      </c>
+      <c r="H18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1132,18 +1619,30 @@
       <c r="D23" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -1156,8 +1655,21 @@
       <c r="D29">
         <v>6</v>
       </c>
+      <c r="E29" t="s">
+        <v>58</v>
+      </c>
+      <c r="F29" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adds Quantitative Data - UX 1 2 3
</commit_message>
<xml_diff>
--- a/docs/user study/results/UX 2.xlsx
+++ b/docs/user study/results/UX 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Varma\Documents\GitHub\MSAT-UI\docs\user study\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33B3E9B3-DC5B-43F5-AD3C-D67FDEEB0CA3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4A0130-7728-4DB6-AB93-9BE3CCC4DD81}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="RQ 3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -580,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1414,7 +1413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0454749A-2141-49B1-B678-977DE214E3EB}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>

</xml_diff>